<commit_message>
Added `Speedup vs NO SFT` column to every Master/Worker group.
</commit_message>
<xml_diff>
--- a/Measurements/centralized_measurements.xlsx
+++ b/Measurements/centralized_measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepo\Desktop\Poli Stuff\An3\Sem1\APD\Proiect MPI\Measurements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA97A600-C717-469E-A63E-0AD8E8C2ED8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99460F0-6501-4F06-A5A3-9A078405FB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{40C3F542-6004-4890-B87F-BE1A1329EA8E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="13">
   <si>
     <t>Large.bmp</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>Chunk Size</t>
+  </si>
+  <si>
+    <t>Speedup vs Serial</t>
+  </si>
+  <si>
+    <t>Speedup vs NO SFT</t>
   </si>
 </sst>
 </file>
@@ -140,7 +146,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -326,10 +332,204 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -338,77 +538,6 @@
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -417,79 +546,12 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -500,6 +562,32 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -509,8 +597,8 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -518,81 +606,27 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
+      <right style="thin">
+        <color auto="1"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -600,48 +634,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -665,7 +699,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -674,61 +708,79 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1074,114 +1126,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FF8C66-6399-4A17-9803-C0E865CC4D86}">
-  <dimension ref="A1:Z19"/>
+  <dimension ref="A1:AH40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+      <selection activeCell="AC23" sqref="AC23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="17" width="9.140625" style="1"/>
-    <col min="18" max="18" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="25" width="9.140625" style="1"/>
-    <col min="26" max="26" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="38" t="s">
+    <row r="1" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="41" t="s">
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="42"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="41" t="s">
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="W2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="42"/>
-      <c r="U2" s="42"/>
-      <c r="V2" s="42"/>
-      <c r="W2" s="42"/>
-      <c r="X2" s="42"/>
-      <c r="Y2" s="42"/>
-      <c r="Z2" s="43"/>
-    </row>
-    <row r="3" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="39"/>
-      <c r="C3" s="30" t="s">
+      <c r="X2" s="34"/>
+      <c r="Y2" s="34"/>
+      <c r="Z2" s="34"/>
+      <c r="AA2" s="34"/>
+      <c r="AB2" s="34"/>
+      <c r="AC2" s="34"/>
+      <c r="AD2" s="34"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+    </row>
+    <row r="3" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="31"/>
+      <c r="C3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="36"/>
-      <c r="F3" s="35" t="s">
+      <c r="E3" s="39"/>
+      <c r="F3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="32" t="s">
+      <c r="G3" s="38"/>
+      <c r="H3" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="30" t="s">
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="35" t="s">
+      <c r="N3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="36"/>
-      <c r="N3" s="35" t="s">
+      <c r="O3" s="39"/>
+      <c r="P3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="37"/>
-      <c r="P3" s="32" t="s">
+      <c r="Q3" s="38"/>
+      <c r="R3" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="34"/>
-      <c r="S3" s="30" t="s">
+      <c r="S3" s="42"/>
+      <c r="T3" s="42"/>
+      <c r="U3" s="43"/>
+      <c r="V3" s="31"/>
+      <c r="W3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="T3" s="35" t="s">
+      <c r="X3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="36"/>
-      <c r="V3" s="35" t="s">
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="W3" s="37"/>
-      <c r="X3" s="32" t="s">
+      <c r="AA3" s="38"/>
+      <c r="AB3" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="Y3" s="33"/>
-      <c r="Z3" s="34"/>
-    </row>
-    <row r="4" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="40"/>
-      <c r="C4" s="31"/>
+      <c r="AC3" s="42"/>
+      <c r="AD3" s="42"/>
+      <c r="AE3" s="43"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+    </row>
+    <row r="4" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="32"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="26" t="s">
         <v>7</v>
       </c>
@@ -1198,18 +1292,16 @@
         <v>7</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="31"/>
-      <c r="L4" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4" s="27" t="s">
-        <v>8</v>
-      </c>
+      <c r="L4" s="32"/>
+      <c r="M4" s="36"/>
       <c r="N4" s="26" t="s">
         <v>7</v>
       </c>
@@ -1219,36 +1311,52 @@
       <c r="P4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="Q4" s="28" t="s">
+      <c r="Q4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="R4" s="27" t="s">
+      <c r="R4" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="S4" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="T4" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="U4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="S4" s="31"/>
-      <c r="T4" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="U4" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="V4" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="W4" s="29" t="s">
-        <v>8</v>
-      </c>
+      <c r="V4" s="32"/>
+      <c r="W4" s="36"/>
       <c r="X4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="Y4" s="28" t="s">
+      <c r="Y4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="Z4" s="27" t="s">
+      <c r="Z4" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA4" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB4" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC4" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD4" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE4" s="27" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+    </row>
+    <row r="5" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B5" s="25">
         <v>2</v>
       </c>
@@ -1267,65 +1375,86 @@
       <c r="G5" s="23">
         <v>6.6323090000000002</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="47">
         <v>0.90600000000000003</v>
       </c>
-      <c r="I5" s="24">
+      <c r="I5" s="48">
         <v>4.7582769999999996</v>
       </c>
-      <c r="J5" s="22">
+      <c r="J5" s="48">
+        <f xml:space="preserve"> F5 / H5</f>
+        <v>0.717439293598234</v>
+      </c>
+      <c r="K5" s="49">
         <v>925</v>
       </c>
-      <c r="K5" s="20">
+      <c r="L5" s="25">
+        <v>2</v>
+      </c>
+      <c r="M5" s="20">
         <v>10.749000000000001</v>
       </c>
-      <c r="L5" s="21">
+      <c r="N5" s="21">
         <v>1.3280000000000001</v>
       </c>
-      <c r="M5" s="22">
+      <c r="O5" s="22">
         <v>8.0941259999999993</v>
       </c>
-      <c r="N5" s="21">
+      <c r="P5" s="21">
         <v>1.6539999999999999</v>
       </c>
-      <c r="O5" s="23">
+      <c r="Q5" s="23">
         <v>6.4987909999999998</v>
       </c>
-      <c r="P5" s="21">
+      <c r="R5" s="21">
         <v>2.3660000000000001</v>
       </c>
-      <c r="Q5" s="24">
+      <c r="S5" s="24">
         <v>4.5431109999999997</v>
       </c>
-      <c r="R5" s="22">
+      <c r="T5" s="48">
+        <f xml:space="preserve"> P5 / R5</f>
+        <v>0.69907016060862204</v>
+      </c>
+      <c r="U5" s="44">
         <v>150</v>
       </c>
-      <c r="S5" s="20">
+      <c r="V5" s="25">
+        <v>2</v>
+      </c>
+      <c r="W5" s="20">
         <v>35.465000000000003</v>
       </c>
-      <c r="T5" s="21">
+      <c r="X5" s="21">
         <v>4.4859999999999998</v>
       </c>
-      <c r="U5" s="22">
+      <c r="Y5" s="22">
         <v>7.9057069999999996</v>
       </c>
-      <c r="V5" s="21">
+      <c r="Z5" s="21">
         <v>5.1040000000000001</v>
       </c>
-      <c r="W5" s="23">
+      <c r="AA5" s="23">
         <v>6.9484719999999998</v>
       </c>
-      <c r="X5" s="21">
+      <c r="AB5" s="21">
         <v>7.77</v>
       </c>
-      <c r="Y5" s="24">
+      <c r="AC5" s="24">
         <v>4.5643500000000001</v>
       </c>
-      <c r="Z5" s="22">
+      <c r="AD5" s="48">
+        <f xml:space="preserve"> Z5 / AB5</f>
+        <v>0.65688545688545696</v>
+      </c>
+      <c r="AE5" s="44">
         <v>955</v>
       </c>
-    </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+    </row>
+    <row r="6" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B6" s="18">
         <v>3</v>
       </c>
@@ -1350,59 +1479,80 @@
       <c r="I6" s="15">
         <v>6.6217879999999996</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="24">
+        <f xml:space="preserve"> F6 / H6</f>
+        <v>1.0922844175491679</v>
+      </c>
+      <c r="K6" s="45">
         <v>715</v>
       </c>
-      <c r="K6" s="16">
+      <c r="L6" s="18">
+        <v>3</v>
+      </c>
+      <c r="M6" s="16">
         <v>10.92</v>
       </c>
-      <c r="L6" s="9">
+      <c r="N6" s="9">
         <v>1.37</v>
       </c>
-      <c r="M6" s="10">
+      <c r="O6" s="10">
         <v>7.9708019999999999</v>
       </c>
-      <c r="N6" s="9">
+      <c r="P6" s="9">
         <v>1.647</v>
       </c>
-      <c r="O6" s="13">
+      <c r="Q6" s="13">
         <v>6.6302380000000003</v>
       </c>
-      <c r="P6" s="9">
+      <c r="R6" s="9">
         <v>1.64</v>
       </c>
-      <c r="Q6" s="15">
+      <c r="S6" s="15">
         <v>6.6585359999999998</v>
       </c>
-      <c r="R6" s="10">
+      <c r="T6" s="15">
+        <f xml:space="preserve"> P6 / R6</f>
+        <v>1.0042682926829269</v>
+      </c>
+      <c r="U6" s="45">
         <v>450</v>
       </c>
-      <c r="S6" s="16">
+      <c r="V6" s="18">
+        <v>3</v>
+      </c>
+      <c r="W6" s="16">
         <v>35.912999999999997</v>
       </c>
-      <c r="T6" s="9">
+      <c r="X6" s="9">
         <v>4.3860000000000001</v>
       </c>
-      <c r="U6" s="10">
+      <c r="Y6" s="10">
         <v>8.1880980000000001</v>
       </c>
-      <c r="V6" s="9">
+      <c r="Z6" s="9">
         <v>5.18</v>
       </c>
-      <c r="W6" s="13">
+      <c r="AA6" s="13">
         <v>6.9330109999999996</v>
       </c>
-      <c r="X6" s="9">
+      <c r="AB6" s="9">
         <v>5.4359999999999999</v>
       </c>
-      <c r="Y6" s="15">
+      <c r="AC6" s="15">
         <v>6.6065120000000004</v>
       </c>
-      <c r="Z6" s="10">
+      <c r="AD6" s="15">
+        <f xml:space="preserve"> Z6 / AB6</f>
+        <v>0.95290654893303894</v>
+      </c>
+      <c r="AE6" s="45">
         <v>915</v>
       </c>
-    </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+    </row>
+    <row r="7" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B7" s="18">
         <v>4</v>
       </c>
@@ -1427,59 +1577,80 @@
       <c r="I7" s="15">
         <v>7.8273380000000001</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="24">
+        <f t="shared" ref="J7:J18" si="0" xml:space="preserve"> F7 / H7</f>
+        <v>1.2715827338129495</v>
+      </c>
+      <c r="K7" s="45">
         <v>140</v>
       </c>
-      <c r="K7" s="16">
+      <c r="L7" s="18">
+        <v>4</v>
+      </c>
+      <c r="M7" s="16">
         <v>10.824999999999999</v>
       </c>
-      <c r="L7" s="9">
+      <c r="N7" s="9">
         <v>1.3660000000000001</v>
       </c>
-      <c r="M7" s="10">
+      <c r="O7" s="10">
         <v>7.9245979999999996</v>
       </c>
-      <c r="N7" s="9">
+      <c r="P7" s="9">
         <v>1.6419999999999999</v>
       </c>
-      <c r="O7" s="13">
+      <c r="Q7" s="13">
         <v>6.5925700000000003</v>
       </c>
-      <c r="P7" s="9">
+      <c r="R7" s="9">
         <v>1.365</v>
       </c>
-      <c r="Q7" s="15">
+      <c r="S7" s="15">
         <v>7.9304030000000001</v>
       </c>
-      <c r="R7" s="10">
+      <c r="T7" s="15">
+        <f t="shared" ref="T7:T18" si="1" xml:space="preserve"> P7 / R7</f>
+        <v>1.2029304029304029</v>
+      </c>
+      <c r="U7" s="45">
         <v>545</v>
       </c>
-      <c r="S7" s="16">
+      <c r="V7" s="18">
+        <v>4</v>
+      </c>
+      <c r="W7" s="16">
         <v>35.493000000000002</v>
       </c>
-      <c r="T7" s="9">
+      <c r="X7" s="9">
         <v>4.0190000000000001</v>
       </c>
-      <c r="U7" s="10">
+      <c r="Y7" s="10">
         <v>8.8313020000000009</v>
       </c>
-      <c r="V7" s="9">
+      <c r="Z7" s="9">
         <v>5.23</v>
       </c>
-      <c r="W7" s="13">
+      <c r="AA7" s="13">
         <v>6.7864240000000002</v>
       </c>
-      <c r="X7" s="9">
+      <c r="AB7" s="9">
         <v>4.4630000000000001</v>
       </c>
-      <c r="Y7" s="15">
+      <c r="AC7" s="15">
         <v>7.9527219999999996</v>
       </c>
-      <c r="Z7" s="10">
+      <c r="AD7" s="15">
+        <f t="shared" ref="AD7:AD18" si="2" xml:space="preserve"> Z7 / AB7</f>
+        <v>1.1718574949585481</v>
+      </c>
+      <c r="AE7" s="45">
         <v>325</v>
       </c>
-    </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+    </row>
+    <row r="8" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B8" s="18">
         <v>5</v>
       </c>
@@ -1504,59 +1675,80 @@
       <c r="I8" s="15">
         <v>8.3396589999999993</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="24">
+        <f t="shared" si="0"/>
+        <v>1.2182163187855788</v>
+      </c>
+      <c r="K8" s="45">
         <v>45</v>
       </c>
-      <c r="K8" s="16">
+      <c r="L8" s="18">
+        <v>5</v>
+      </c>
+      <c r="M8" s="16">
         <v>10.87</v>
       </c>
-      <c r="L8" s="9">
+      <c r="N8" s="9">
         <v>1.3109999999999999</v>
       </c>
-      <c r="M8" s="10">
+      <c r="O8" s="10">
         <v>8.2913800000000002</v>
       </c>
-      <c r="N8" s="9">
+      <c r="P8" s="9">
         <v>1.54</v>
       </c>
-      <c r="O8" s="13">
+      <c r="Q8" s="13">
         <v>7.0584410000000002</v>
       </c>
-      <c r="P8" s="9">
+      <c r="R8" s="9">
         <v>1.333</v>
       </c>
-      <c r="Q8" s="15">
+      <c r="S8" s="15">
         <v>8.1545389999999998</v>
       </c>
-      <c r="R8" s="10">
+      <c r="T8" s="15">
+        <f t="shared" si="1"/>
+        <v>1.1552888222055515</v>
+      </c>
+      <c r="U8" s="45">
         <v>335</v>
       </c>
-      <c r="S8" s="16">
+      <c r="V8" s="18">
+        <v>5</v>
+      </c>
+      <c r="W8" s="16">
         <v>36.036999999999999</v>
       </c>
-      <c r="T8" s="9">
+      <c r="X8" s="9">
         <v>4.09</v>
       </c>
-      <c r="U8" s="10">
+      <c r="Y8" s="10">
         <v>8.8110029999999995</v>
       </c>
-      <c r="V8" s="9">
+      <c r="Z8" s="9">
         <v>5.2919999999999998</v>
       </c>
-      <c r="W8" s="13">
+      <c r="AA8" s="13">
         <v>6.8097130000000003</v>
       </c>
-      <c r="X8" s="9">
+      <c r="AB8" s="9">
         <v>4.3609999999999998</v>
       </c>
-      <c r="Y8" s="15">
+      <c r="AC8" s="15">
         <v>8.2634720000000002</v>
       </c>
-      <c r="Z8" s="10">
+      <c r="AD8" s="15">
+        <f t="shared" si="2"/>
+        <v>1.2134831460674158</v>
+      </c>
+      <c r="AE8" s="45">
         <v>290</v>
       </c>
-    </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+    </row>
+    <row r="9" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B9" s="18">
         <v>6</v>
       </c>
@@ -1581,59 +1773,80 @@
       <c r="I9" s="15">
         <v>7.3139539999999998</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="24">
+        <f xml:space="preserve"> F9 / H9</f>
+        <v>1.1511627906976745</v>
+      </c>
+      <c r="K9" s="45">
         <v>85</v>
       </c>
-      <c r="K9" s="16">
+      <c r="L9" s="18">
+        <v>6</v>
+      </c>
+      <c r="M9" s="16">
         <v>10.896000000000001</v>
       </c>
-      <c r="L9" s="9">
+      <c r="N9" s="9">
         <v>1.331</v>
       </c>
-      <c r="M9" s="10">
+      <c r="O9" s="10">
         <v>8.1863250000000001</v>
       </c>
-      <c r="N9" s="9">
+      <c r="P9" s="9">
         <v>1.653</v>
       </c>
-      <c r="O9" s="13">
+      <c r="Q9" s="13">
         <v>6.5916519999999998</v>
       </c>
-      <c r="P9" s="9">
+      <c r="R9" s="9">
         <v>1.492</v>
       </c>
-      <c r="Q9" s="15">
+      <c r="S9" s="15">
         <v>7.3029479999999998</v>
       </c>
-      <c r="R9" s="10">
+      <c r="T9" s="15">
+        <f t="shared" si="1"/>
+        <v>1.1079088471849867</v>
+      </c>
+      <c r="U9" s="45">
         <v>20</v>
       </c>
-      <c r="S9" s="16">
+      <c r="V9" s="18">
+        <v>6</v>
+      </c>
+      <c r="W9" s="16">
         <v>35.826000000000001</v>
       </c>
-      <c r="T9" s="9">
+      <c r="X9" s="9">
         <v>4.4530000000000003</v>
       </c>
-      <c r="U9" s="10">
+      <c r="Y9" s="10">
         <v>8.045363</v>
       </c>
-      <c r="V9" s="9">
+      <c r="Z9" s="9">
         <v>5.6479999999999997</v>
       </c>
-      <c r="W9" s="13">
+      <c r="AA9" s="13">
         <v>6.3431300000000004</v>
       </c>
-      <c r="X9" s="9">
+      <c r="AB9" s="9">
         <v>4.944</v>
       </c>
-      <c r="Y9" s="15">
+      <c r="AC9" s="15">
         <v>7.246359</v>
       </c>
-      <c r="Z9" s="10">
+      <c r="AD9" s="15">
+        <f t="shared" si="2"/>
+        <v>1.1423948220064724</v>
+      </c>
+      <c r="AE9" s="45">
         <v>250</v>
       </c>
-    </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+    </row>
+    <row r="10" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B10" s="18">
         <v>7</v>
       </c>
@@ -1658,59 +1871,80 @@
       <c r="I10" s="15">
         <v>8.3339669999999995</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="24">
+        <f t="shared" si="0"/>
+        <v>1.2099236641221374</v>
+      </c>
+      <c r="K10" s="45">
         <v>25</v>
       </c>
-      <c r="K10" s="16">
+      <c r="L10" s="18">
+        <v>7</v>
+      </c>
+      <c r="M10" s="16">
         <v>10.766</v>
       </c>
-      <c r="L10" s="9">
+      <c r="N10" s="9">
         <v>1.294</v>
       </c>
-      <c r="M10" s="10">
+      <c r="O10" s="10">
         <v>8.3199389999999998</v>
       </c>
-      <c r="N10" s="9">
+      <c r="P10" s="9">
         <v>1.6060000000000001</v>
       </c>
-      <c r="O10" s="13">
+      <c r="Q10" s="13">
         <v>6.7036110000000004</v>
       </c>
-      <c r="P10" s="9">
+      <c r="R10" s="9">
         <v>1.2769999999999999</v>
       </c>
-      <c r="Q10" s="15">
+      <c r="S10" s="15">
         <v>8.4306970000000003</v>
       </c>
-      <c r="R10" s="10">
+      <c r="T10" s="15">
+        <f t="shared" si="1"/>
+        <v>1.2576350822239626</v>
+      </c>
+      <c r="U10" s="45">
         <v>30</v>
       </c>
-      <c r="S10" s="16">
+      <c r="V10" s="18">
+        <v>7</v>
+      </c>
+      <c r="W10" s="16">
         <v>35.491</v>
       </c>
-      <c r="T10" s="9">
+      <c r="X10" s="9">
         <v>4.1120000000000001</v>
       </c>
-      <c r="U10" s="10">
+      <c r="Y10" s="10">
         <v>8.6310800000000008</v>
       </c>
-      <c r="V10" s="9">
+      <c r="Z10" s="9">
         <v>5.2569999999999997</v>
       </c>
-      <c r="W10" s="13">
+      <c r="AA10" s="13">
         <v>6.7511890000000001</v>
       </c>
-      <c r="X10" s="9">
+      <c r="AB10" s="9">
         <v>4.1740000000000004</v>
       </c>
-      <c r="Y10" s="15">
+      <c r="AC10" s="15">
         <v>8.5028749999999995</v>
       </c>
-      <c r="Z10" s="10">
+      <c r="AD10" s="15">
+        <f t="shared" si="2"/>
+        <v>1.2594633445136558</v>
+      </c>
+      <c r="AE10" s="45">
         <v>150</v>
       </c>
-    </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+    </row>
+    <row r="11" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B11" s="18">
         <v>8</v>
       </c>
@@ -1735,59 +1969,80 @@
       <c r="I11" s="15">
         <v>9.3677440000000001</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="24">
+        <f t="shared" si="0"/>
+        <v>1.3634408602150536</v>
+      </c>
+      <c r="K11" s="45">
         <v>50</v>
       </c>
-      <c r="K11" s="16">
+      <c r="L11" s="18">
+        <v>8</v>
+      </c>
+      <c r="M11" s="16">
         <v>10.813000000000001</v>
       </c>
-      <c r="L11" s="2">
+      <c r="N11" s="2">
         <v>1.246</v>
       </c>
-      <c r="M11" s="3">
+      <c r="O11" s="3">
         <v>8.6781710000000007</v>
       </c>
-      <c r="N11" s="2">
+      <c r="P11" s="2">
         <v>1.5349999999999999</v>
       </c>
-      <c r="O11" s="4">
+      <c r="Q11" s="4">
         <v>7.0442989999999996</v>
       </c>
-      <c r="P11" s="9">
+      <c r="R11" s="9">
         <v>1.1519999999999999</v>
       </c>
-      <c r="Q11" s="15">
+      <c r="S11" s="15">
         <v>9.3862850000000009</v>
       </c>
-      <c r="R11" s="10">
+      <c r="T11" s="15">
+        <f t="shared" si="1"/>
+        <v>1.3324652777777779</v>
+      </c>
+      <c r="U11" s="45">
         <v>75</v>
       </c>
-      <c r="S11" s="16">
+      <c r="V11" s="18">
+        <v>8</v>
+      </c>
+      <c r="W11" s="16">
         <v>35.561</v>
       </c>
-      <c r="T11" s="9">
+      <c r="X11" s="9">
         <v>3.843</v>
       </c>
-      <c r="U11" s="10">
+      <c r="Y11" s="10">
         <v>9.2534469999999995</v>
       </c>
-      <c r="V11" s="9">
+      <c r="Z11" s="9">
         <v>5.0190000000000001</v>
       </c>
-      <c r="W11" s="13">
+      <c r="AA11" s="13">
         <v>7.0852760000000004</v>
       </c>
-      <c r="X11" s="9">
+      <c r="AB11" s="9">
         <v>3.8130000000000002</v>
       </c>
-      <c r="Y11" s="15">
+      <c r="AC11" s="15">
         <v>9.3262520000000002</v>
       </c>
-      <c r="Z11" s="10">
+      <c r="AD11" s="15">
+        <f t="shared" si="2"/>
+        <v>1.3162863886703382</v>
+      </c>
+      <c r="AE11" s="45">
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
+    </row>
+    <row r="12" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B12" s="18">
         <v>9</v>
       </c>
@@ -1812,59 +2067,80 @@
       <c r="I12" s="15">
         <v>6.4425059999999998</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="24">
+        <f t="shared" si="0"/>
+        <v>1.1659388646288209</v>
+      </c>
+      <c r="K12" s="45">
         <v>20</v>
       </c>
-      <c r="K12" s="16">
+      <c r="L12" s="18">
+        <v>9</v>
+      </c>
+      <c r="M12" s="16">
         <v>10.911</v>
       </c>
-      <c r="L12" s="9">
+      <c r="N12" s="9">
         <v>1.536</v>
       </c>
-      <c r="M12" s="10">
+      <c r="O12" s="10">
         <v>7.1035149999999998</v>
       </c>
-      <c r="N12" s="9">
+      <c r="P12" s="9">
         <v>1.9790000000000001</v>
       </c>
-      <c r="O12" s="13">
+      <c r="Q12" s="13">
         <v>5.5133900000000002</v>
       </c>
-      <c r="P12" s="9">
+      <c r="R12" s="9">
         <v>1.69</v>
       </c>
-      <c r="Q12" s="15">
+      <c r="S12" s="15">
         <v>6.4562140000000001</v>
       </c>
-      <c r="R12" s="10">
+      <c r="T12" s="15">
+        <f t="shared" si="1"/>
+        <v>1.1710059171597633</v>
+      </c>
+      <c r="U12" s="45">
         <v>20</v>
       </c>
-      <c r="S12" s="16">
+      <c r="V12" s="18">
+        <v>9</v>
+      </c>
+      <c r="W12" s="16">
         <v>36.143999999999998</v>
       </c>
-      <c r="T12" s="9">
+      <c r="X12" s="9">
         <v>5.1029999999999998</v>
       </c>
-      <c r="U12" s="10">
+      <c r="Y12" s="10">
         <v>7.0828930000000003</v>
       </c>
-      <c r="V12" s="9">
+      <c r="Z12" s="9">
         <v>6.5250000000000004</v>
       </c>
-      <c r="W12" s="13">
+      <c r="AA12" s="13">
         <v>5.5393100000000004</v>
       </c>
-      <c r="X12" s="9">
+      <c r="AB12" s="9">
         <v>5.6379999999999999</v>
       </c>
-      <c r="Y12" s="15">
+      <c r="AC12" s="15">
         <v>6.4107839999999996</v>
       </c>
-      <c r="Z12" s="10">
+      <c r="AD12" s="15">
+        <f t="shared" si="2"/>
+        <v>1.1573252926569706</v>
+      </c>
+      <c r="AE12" s="45">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+    </row>
+    <row r="13" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B13" s="18">
         <v>10</v>
       </c>
@@ -1889,59 +2165,80 @@
       <c r="I13" s="15">
         <v>7.1319210000000002</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="24">
+        <f t="shared" si="0"/>
+        <v>1.2035830618892509</v>
+      </c>
+      <c r="K13" s="45">
         <v>20</v>
       </c>
-      <c r="K13" s="16">
+      <c r="L13" s="18">
+        <v>10</v>
+      </c>
+      <c r="M13" s="16">
         <v>10.835000000000001</v>
       </c>
-      <c r="L13" s="9">
+      <c r="N13" s="9">
         <v>1.407</v>
       </c>
-      <c r="M13" s="10">
+      <c r="O13" s="10">
         <v>7.7007830000000004</v>
       </c>
-      <c r="N13" s="9">
+      <c r="P13" s="9">
         <v>1.8360000000000001</v>
       </c>
-      <c r="O13" s="13">
+      <c r="Q13" s="13">
         <v>5.9014160000000002</v>
       </c>
-      <c r="P13" s="9">
+      <c r="R13" s="9">
         <v>1.5189999999999999</v>
       </c>
-      <c r="Q13" s="15">
+      <c r="S13" s="15">
         <v>7.1329820000000002</v>
       </c>
-      <c r="R13" s="10">
+      <c r="T13" s="15">
+        <f t="shared" si="1"/>
+        <v>1.2086899275839369</v>
+      </c>
+      <c r="U13" s="45">
         <v>25</v>
       </c>
-      <c r="S13" s="16">
+      <c r="V13" s="18">
+        <v>10</v>
+      </c>
+      <c r="W13" s="16">
         <v>36.360999999999997</v>
       </c>
-      <c r="T13" s="9">
+      <c r="X13" s="9">
         <v>5.0730000000000004</v>
       </c>
-      <c r="U13" s="10">
+      <c r="Y13" s="10">
         <v>7.1675529999999998</v>
       </c>
-      <c r="V13" s="9">
+      <c r="Z13" s="9">
         <v>6.3090000000000002</v>
       </c>
-      <c r="W13" s="13">
+      <c r="AA13" s="13">
         <v>5.7633539999999996</v>
       </c>
-      <c r="X13" s="9">
+      <c r="AB13" s="9">
         <v>5.0629999999999997</v>
       </c>
-      <c r="Y13" s="15">
+      <c r="AC13" s="15">
         <v>7.1817099999999998</v>
       </c>
-      <c r="Z13" s="10">
+      <c r="AD13" s="15">
+        <f t="shared" si="2"/>
+        <v>1.2460991507011654</v>
+      </c>
+      <c r="AE13" s="45">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="1"/>
+      <c r="AH13" s="1"/>
+    </row>
+    <row r="14" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B14" s="18">
         <v>11</v>
       </c>
@@ -1966,59 +2263,80 @@
       <c r="I14" s="15">
         <v>7.8467010000000004</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="24">
+        <f t="shared" si="0"/>
+        <v>1.2549019607843135</v>
+      </c>
+      <c r="K14" s="45">
         <v>10</v>
       </c>
-      <c r="K14" s="16">
+      <c r="L14" s="18">
+        <v>11</v>
+      </c>
+      <c r="M14" s="16">
         <v>10.84</v>
       </c>
-      <c r="L14" s="9">
+      <c r="N14" s="9">
         <v>1.38</v>
       </c>
-      <c r="M14" s="10">
+      <c r="O14" s="10">
         <v>7.855073</v>
       </c>
-      <c r="N14" s="9">
+      <c r="P14" s="9">
         <v>1.7569999999999999</v>
       </c>
-      <c r="O14" s="13">
+      <c r="Q14" s="13">
         <v>6.1696070000000001</v>
       </c>
-      <c r="P14" s="9">
+      <c r="R14" s="9">
         <v>1.387</v>
       </c>
-      <c r="Q14" s="15">
+      <c r="S14" s="15">
         <v>7.815429</v>
       </c>
-      <c r="R14" s="10">
+      <c r="T14" s="15">
+        <f t="shared" si="1"/>
+        <v>1.26676279740447</v>
+      </c>
+      <c r="U14" s="45">
         <v>25</v>
       </c>
-      <c r="S14" s="16">
+      <c r="V14" s="18">
+        <v>11</v>
+      </c>
+      <c r="W14" s="16">
         <v>36.155999999999999</v>
       </c>
-      <c r="T14" s="9">
+      <c r="X14" s="9">
         <v>4.3019999999999996</v>
       </c>
-      <c r="U14" s="10">
+      <c r="Y14" s="10">
         <v>8.4044629999999998</v>
       </c>
-      <c r="V14" s="9">
+      <c r="Z14" s="9">
         <v>5.7220000000000004</v>
       </c>
-      <c r="W14" s="13">
+      <c r="AA14" s="13">
         <v>6.3187699999999998</v>
       </c>
-      <c r="X14" s="9">
+      <c r="AB14" s="9">
         <v>4.6040000000000001</v>
       </c>
-      <c r="Y14" s="15">
+      <c r="AC14" s="15">
         <v>7.8531709999999997</v>
       </c>
-      <c r="Z14" s="10">
+      <c r="AD14" s="15">
+        <f t="shared" si="2"/>
+        <v>1.242832319721981</v>
+      </c>
+      <c r="AE14" s="45">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="1"/>
+      <c r="AH14" s="1"/>
+    </row>
+    <row r="15" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B15" s="18">
         <v>12</v>
       </c>
@@ -2043,59 +2361,80 @@
       <c r="I15" s="15">
         <v>8.3570039999999999</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="24">
+        <f t="shared" si="0"/>
+        <v>1.2917466410748562</v>
+      </c>
+      <c r="K15" s="45">
         <v>10</v>
       </c>
-      <c r="K15" s="16">
+      <c r="L15" s="18">
+        <v>12</v>
+      </c>
+      <c r="M15" s="16">
         <v>10.788</v>
       </c>
-      <c r="L15" s="9">
+      <c r="N15" s="9">
         <v>1.2729999999999999</v>
       </c>
-      <c r="M15" s="10">
+      <c r="O15" s="10">
         <v>8.4744700000000002</v>
       </c>
-      <c r="N15" s="9">
+      <c r="P15" s="9">
         <v>1.659</v>
       </c>
-      <c r="O15" s="13">
+      <c r="Q15" s="13">
         <v>6.502713</v>
       </c>
-      <c r="P15" s="9">
+      <c r="R15" s="9">
         <v>1.2789999999999999</v>
       </c>
-      <c r="Q15" s="15">
+      <c r="S15" s="15">
         <v>8.4347139999999996</v>
       </c>
-      <c r="R15" s="10">
+      <c r="T15" s="15">
+        <f t="shared" si="1"/>
+        <v>1.297107114933542</v>
+      </c>
+      <c r="U15" s="45">
         <v>20</v>
       </c>
-      <c r="S15" s="16">
+      <c r="V15" s="18">
+        <v>12</v>
+      </c>
+      <c r="W15" s="16">
         <v>35.616999999999997</v>
       </c>
-      <c r="T15" s="9">
+      <c r="X15" s="9">
         <v>4.157</v>
       </c>
-      <c r="U15" s="10">
+      <c r="Y15" s="10">
         <v>8.5679569999999998</v>
       </c>
-      <c r="V15" s="9">
+      <c r="Z15" s="9">
         <v>5.4039999999999999</v>
       </c>
-      <c r="W15" s="13">
+      <c r="AA15" s="13">
         <v>6.590859</v>
       </c>
-      <c r="X15" s="9">
+      <c r="AB15" s="9">
         <v>4.2720000000000002</v>
       </c>
-      <c r="Y15" s="15">
+      <c r="AC15" s="15">
         <v>8.337313</v>
       </c>
-      <c r="Z15" s="10">
+      <c r="AD15" s="15">
+        <f t="shared" si="2"/>
+        <v>1.2649812734082395</v>
+      </c>
+      <c r="AE15" s="45">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+    </row>
+    <row r="16" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B16" s="18">
         <v>13</v>
       </c>
@@ -2120,59 +2459,80 @@
       <c r="I16" s="15">
         <v>8.9567890000000006</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="24">
+        <f t="shared" si="0"/>
+        <v>1.419753086419753</v>
+      </c>
+      <c r="K16" s="45">
         <v>20</v>
       </c>
-      <c r="K16" s="16">
+      <c r="L16" s="18">
+        <v>13</v>
+      </c>
+      <c r="M16" s="16">
         <v>10.734</v>
       </c>
-      <c r="L16" s="9">
+      <c r="N16" s="9">
         <v>1.2929999999999999</v>
       </c>
-      <c r="M16" s="10">
+      <c r="O16" s="10">
         <v>8.3016240000000003</v>
       </c>
-      <c r="N16" s="9">
+      <c r="P16" s="9">
         <v>1.61</v>
       </c>
-      <c r="O16" s="13">
+      <c r="Q16" s="13">
         <v>6.6670809999999996</v>
       </c>
-      <c r="P16" s="9">
+      <c r="R16" s="9">
         <v>1.1919999999999999</v>
       </c>
-      <c r="Q16" s="15">
+      <c r="S16" s="15">
         <v>9.0050340000000002</v>
       </c>
-      <c r="R16" s="10">
+      <c r="T16" s="15">
+        <f t="shared" si="1"/>
+        <v>1.3506711409395975</v>
+      </c>
+      <c r="U16" s="45">
         <v>20</v>
       </c>
-      <c r="S16" s="16">
+      <c r="V16" s="18">
+        <v>13</v>
+      </c>
+      <c r="W16" s="16">
         <v>35.707000000000001</v>
       </c>
-      <c r="T16" s="9">
+      <c r="X16" s="9">
         <v>4.0650000000000004</v>
       </c>
-      <c r="U16" s="10">
+      <c r="Y16" s="10">
         <v>8.7840100000000003</v>
       </c>
-      <c r="V16" s="9">
+      <c r="Z16" s="9">
         <v>5.2640000000000002</v>
       </c>
-      <c r="W16" s="13">
+      <c r="AA16" s="13">
         <v>6.7832439999999998</v>
       </c>
-      <c r="X16" s="9">
+      <c r="AB16" s="9">
         <v>4.0389999999999997</v>
       </c>
-      <c r="Y16" s="15">
+      <c r="AC16" s="15">
         <v>8.8405550000000002</v>
       </c>
-      <c r="Z16" s="10">
+      <c r="AD16" s="15">
+        <f t="shared" si="2"/>
+        <v>1.3032928942807627</v>
+      </c>
+      <c r="AE16" s="45">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="1"/>
+      <c r="AH16" s="1"/>
+    </row>
+    <row r="17" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B17" s="18">
         <v>14</v>
       </c>
@@ -2197,59 +2557,80 @@
       <c r="I17" s="15">
         <v>9.1572329999999997</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="24">
+        <f t="shared" si="0"/>
+        <v>1.3836477987421385</v>
+      </c>
+      <c r="K17" s="45">
         <v>15</v>
       </c>
-      <c r="K17" s="16">
+      <c r="L17" s="18">
+        <v>14</v>
+      </c>
+      <c r="M17" s="16">
         <v>10.782</v>
       </c>
-      <c r="L17" s="9">
+      <c r="N17" s="9">
         <v>1.3280000000000001</v>
       </c>
-      <c r="M17" s="10">
+      <c r="O17" s="10">
         <v>8.1189750000000007</v>
       </c>
-      <c r="N17" s="9">
+      <c r="P17" s="9">
         <v>1.5649999999999999</v>
       </c>
-      <c r="O17" s="13">
+      <c r="Q17" s="13">
         <v>6.8894570000000002</v>
       </c>
-      <c r="P17" s="9">
+      <c r="R17" s="9">
         <v>1.165</v>
       </c>
-      <c r="Q17" s="15">
+      <c r="S17" s="15">
         <v>9.2549360000000007</v>
       </c>
-      <c r="R17" s="10">
+      <c r="T17" s="15">
+        <f t="shared" si="1"/>
+        <v>1.3433476394849784</v>
+      </c>
+      <c r="U17" s="45">
         <v>15</v>
       </c>
-      <c r="S17" s="16">
+      <c r="V17" s="18">
+        <v>14</v>
+      </c>
+      <c r="W17" s="16">
         <v>35.909999999999997</v>
       </c>
-      <c r="T17" s="9">
+      <c r="X17" s="9">
         <v>3.83</v>
       </c>
-      <c r="U17" s="10">
+      <c r="Y17" s="10">
         <v>9.3759789999999992</v>
       </c>
-      <c r="V17" s="9">
+      <c r="Z17" s="9">
         <v>5.2990000000000004</v>
       </c>
-      <c r="W17" s="13">
+      <c r="AA17" s="13">
         <v>6.7767499999999998</v>
       </c>
-      <c r="X17" s="9">
+      <c r="AB17" s="9">
         <v>3.8769999999999998</v>
       </c>
-      <c r="Y17" s="15">
+      <c r="AC17" s="15">
         <v>9.2623160000000002</v>
       </c>
-      <c r="Z17" s="10">
+      <c r="AD17" s="15">
+        <f t="shared" si="2"/>
+        <v>1.3667784369357752</v>
+      </c>
+      <c r="AE17" s="45">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="AF17" s="1"/>
+      <c r="AG17" s="1"/>
+      <c r="AH17" s="1"/>
+    </row>
+    <row r="18" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B18" s="18">
         <v>15</v>
       </c>
@@ -2274,59 +2655,80 @@
       <c r="I18" s="15">
         <v>9.452788</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="24">
+        <f t="shared" si="0"/>
+        <v>1.3819742489270386</v>
+      </c>
+      <c r="K18" s="45">
         <v>15</v>
       </c>
-      <c r="K18" s="16">
+      <c r="L18" s="18">
+        <v>15</v>
+      </c>
+      <c r="M18" s="16">
         <v>10.837</v>
       </c>
-      <c r="L18" s="9">
+      <c r="N18" s="9">
         <v>1.4359999999999999</v>
       </c>
-      <c r="M18" s="10">
+      <c r="O18" s="10">
         <v>7.5466579999999999</v>
       </c>
-      <c r="N18" s="9">
+      <c r="P18" s="9">
         <v>1.5680000000000001</v>
       </c>
-      <c r="O18" s="13">
+      <c r="Q18" s="13">
         <v>6.9113530000000001</v>
       </c>
-      <c r="P18" s="9">
+      <c r="R18" s="9">
         <v>1.123</v>
       </c>
-      <c r="Q18" s="15">
+      <c r="S18" s="15">
         <v>9.6500450000000004</v>
       </c>
-      <c r="R18" s="10">
+      <c r="T18" s="15">
+        <f t="shared" si="1"/>
+        <v>1.3962600178094391</v>
+      </c>
+      <c r="U18" s="45">
         <v>25</v>
       </c>
-      <c r="S18" s="16">
+      <c r="V18" s="18">
+        <v>15</v>
+      </c>
+      <c r="W18" s="16">
         <v>36.334000000000003</v>
       </c>
-      <c r="T18" s="9">
+      <c r="X18" s="9">
         <v>3.8210000000000002</v>
       </c>
-      <c r="U18" s="10">
+      <c r="Y18" s="10">
         <v>9.509029</v>
       </c>
-      <c r="V18" s="9">
+      <c r="Z18" s="9">
         <v>5.032</v>
       </c>
-      <c r="W18" s="13">
+      <c r="AA18" s="13">
         <v>7.2205880000000002</v>
       </c>
-      <c r="X18" s="9">
+      <c r="AB18" s="9">
         <v>3.7480000000000002</v>
       </c>
-      <c r="Y18" s="15">
+      <c r="AC18" s="15">
         <v>9.6942369999999993</v>
       </c>
-      <c r="Z18" s="10">
+      <c r="AD18" s="15">
+        <f t="shared" si="2"/>
+        <v>1.3425827107790822</v>
+      </c>
+      <c r="AE18" s="45">
         <v>75</v>
       </c>
-    </row>
-    <row r="19" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AF18" s="1"/>
+      <c r="AG18" s="1"/>
+      <c r="AH18" s="1"/>
+    </row>
+    <row r="19" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="19">
         <v>16</v>
       </c>
@@ -2351,76 +2753,531 @@
       <c r="I19" s="6">
         <v>9.6409690000000001</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J19" s="6">
+        <f xml:space="preserve"> F19 / H19</f>
+        <v>1.4581497797356828</v>
+      </c>
+      <c r="K19" s="46">
         <v>20</v>
       </c>
-      <c r="K19" s="17">
+      <c r="L19" s="19">
+        <v>16</v>
+      </c>
+      <c r="M19" s="17">
         <v>10.736000000000001</v>
       </c>
-      <c r="L19" s="11">
+      <c r="N19" s="11">
         <v>1.337</v>
       </c>
-      <c r="M19" s="12">
+      <c r="O19" s="12">
         <v>8.0299180000000003</v>
       </c>
-      <c r="N19" s="11">
+      <c r="P19" s="11">
         <v>1.5820000000000001</v>
       </c>
-      <c r="O19" s="14">
+      <c r="Q19" s="14">
         <v>6.786346</v>
       </c>
-      <c r="P19" s="5">
+      <c r="R19" s="5">
         <v>1.0980000000000001</v>
       </c>
-      <c r="Q19" s="6">
+      <c r="S19" s="6">
         <v>9.7777770000000004</v>
       </c>
-      <c r="R19" s="7">
+      <c r="T19" s="6">
+        <f xml:space="preserve"> P19 / R19</f>
+        <v>1.4408014571948997</v>
+      </c>
+      <c r="U19" s="46">
         <v>20</v>
       </c>
-      <c r="S19" s="17">
+      <c r="V19" s="19">
+        <v>16</v>
+      </c>
+      <c r="W19" s="17">
         <v>35.942</v>
       </c>
-      <c r="T19" s="5">
+      <c r="X19" s="5">
         <v>3.6840000000000002</v>
       </c>
-      <c r="U19" s="7">
+      <c r="Y19" s="7">
         <v>9.7562429999999996</v>
       </c>
-      <c r="V19" s="5">
+      <c r="Z19" s="5">
         <v>5.0140000000000002</v>
       </c>
-      <c r="W19" s="8">
+      <c r="AA19" s="8">
         <v>7.168329</v>
       </c>
-      <c r="X19" s="5">
+      <c r="AB19" s="5">
         <v>3.597</v>
       </c>
-      <c r="Y19" s="6">
+      <c r="AC19" s="6">
         <v>9.9922160000000009</v>
       </c>
-      <c r="Z19" s="7">
+      <c r="AD19" s="6">
+        <f xml:space="preserve"> Z19 / AB19</f>
+        <v>1.393939393939394</v>
+      </c>
+      <c r="AE19" s="46">
         <v>40</v>
       </c>
+      <c r="AF19" s="1"/>
+      <c r="AG19" s="1"/>
+      <c r="AH19" s="1"/>
+    </row>
+    <row r="23" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+      <c r="S23"/>
+      <c r="T23"/>
+      <c r="U23"/>
+      <c r="V23"/>
+      <c r="W23"/>
+      <c r="X23"/>
+      <c r="Y23"/>
+    </row>
+    <row r="24" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="Q24"/>
+      <c r="R24"/>
+      <c r="S24"/>
+      <c r="T24"/>
+      <c r="U24"/>
+      <c r="V24"/>
+      <c r="W24"/>
+      <c r="X24"/>
+      <c r="Y24"/>
+    </row>
+    <row r="25" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="Q25"/>
+      <c r="R25"/>
+      <c r="S25"/>
+      <c r="T25"/>
+      <c r="U25"/>
+      <c r="V25"/>
+      <c r="W25"/>
+      <c r="X25"/>
+      <c r="Y25"/>
+    </row>
+    <row r="26" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26"/>
+      <c r="Q26"/>
+      <c r="R26"/>
+      <c r="S26"/>
+      <c r="T26"/>
+      <c r="U26"/>
+      <c r="V26"/>
+      <c r="W26"/>
+      <c r="X26"/>
+      <c r="Y26"/>
+    </row>
+    <row r="27" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
+      <c r="Q27"/>
+      <c r="R27"/>
+      <c r="S27"/>
+      <c r="T27"/>
+      <c r="U27"/>
+      <c r="V27"/>
+      <c r="W27"/>
+      <c r="X27"/>
+      <c r="Y27"/>
+    </row>
+    <row r="28" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="Q28"/>
+      <c r="R28"/>
+      <c r="S28"/>
+      <c r="T28"/>
+      <c r="U28"/>
+      <c r="V28"/>
+      <c r="W28"/>
+      <c r="X28"/>
+      <c r="Y28"/>
+    </row>
+    <row r="29" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29"/>
+      <c r="Q29"/>
+      <c r="R29"/>
+      <c r="S29"/>
+      <c r="T29"/>
+      <c r="U29"/>
+      <c r="V29"/>
+      <c r="W29"/>
+      <c r="X29"/>
+      <c r="Y29"/>
+    </row>
+    <row r="30" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="Q30"/>
+      <c r="R30"/>
+      <c r="S30"/>
+      <c r="T30"/>
+      <c r="U30"/>
+      <c r="V30"/>
+      <c r="W30"/>
+      <c r="X30"/>
+      <c r="Y30"/>
+    </row>
+    <row r="31" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="Q31"/>
+      <c r="R31"/>
+      <c r="S31"/>
+      <c r="T31"/>
+      <c r="U31"/>
+      <c r="V31"/>
+      <c r="W31"/>
+      <c r="X31"/>
+      <c r="Y31"/>
+    </row>
+    <row r="32" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+      <c r="S32"/>
+      <c r="T32"/>
+      <c r="U32"/>
+      <c r="V32"/>
+      <c r="W32"/>
+      <c r="X32"/>
+      <c r="Y32"/>
+    </row>
+    <row r="33" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
+      <c r="S33"/>
+      <c r="T33"/>
+      <c r="U33"/>
+      <c r="V33"/>
+      <c r="W33"/>
+      <c r="X33"/>
+      <c r="Y33"/>
+    </row>
+    <row r="34" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+      <c r="T34"/>
+      <c r="U34"/>
+      <c r="V34"/>
+      <c r="W34"/>
+      <c r="X34"/>
+      <c r="Y34"/>
+    </row>
+    <row r="35" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+      <c r="X35"/>
+      <c r="Y35"/>
+    </row>
+    <row r="36" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+      <c r="U36"/>
+      <c r="V36"/>
+      <c r="W36"/>
+      <c r="X36"/>
+      <c r="Y36"/>
+    </row>
+    <row r="37" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37"/>
+      <c r="Y37"/>
+    </row>
+    <row r="38" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B38"/>
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
+      <c r="Q38"/>
+      <c r="R38"/>
+      <c r="S38"/>
+      <c r="T38"/>
+      <c r="U38"/>
+      <c r="V38"/>
+      <c r="W38"/>
+      <c r="X38"/>
+      <c r="Y38"/>
+    </row>
+    <row r="39" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B39"/>
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39"/>
+      <c r="O39"/>
+      <c r="Q39"/>
+      <c r="R39"/>
+      <c r="S39"/>
+      <c r="T39"/>
+      <c r="U39"/>
+      <c r="V39"/>
+      <c r="W39"/>
+      <c r="X39"/>
+      <c r="Y39"/>
+    </row>
+    <row r="40" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40"/>
+      <c r="O40"/>
+      <c r="Q40"/>
+      <c r="R40"/>
+      <c r="S40"/>
+      <c r="T40"/>
+      <c r="U40"/>
+      <c r="V40"/>
+      <c r="W40"/>
+      <c r="X40"/>
+      <c r="Y40"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="18">
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="M2:U2"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="V2:V4"/>
+    <mergeCell ref="W2:AE2"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AE3"/>
+    <mergeCell ref="C2:K2"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L2:L4"/>
     <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="K2:R2"/>
-    <mergeCell ref="S2:Z2"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="V3:W3"/>
     <mergeCell ref="C3:C4"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="P3:R3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>